<commit_message>
updated codes for new version of paper
</commit_message>
<xml_diff>
--- a/DataFileDescription.xlsx
+++ b/DataFileDescription.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ditong\Dropbox (MIT)\skills\SkillPaper\CodesData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ditong\Dropbox (MIT)\skills\SkillPaper\SkillPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6759F172-A40C-485A-A6C4-4698B4F19B9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E85A2A-3B0B-4734-997D-76D3B12438CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{BB7D513F-C907-4CFD-A1F8-9CA708EEEE7B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
   <si>
     <t>Filename</t>
   </si>
@@ -85,15 +85,9 @@
     <t>small companies: 2010, 2018</t>
   </si>
   <si>
-    <t>lloc1_occ_year_skill_freq.txt</t>
-  </si>
-  <si>
     <t>large locations: 2010, 2018</t>
   </si>
   <si>
-    <t>sloc1_occ_year_skill_freq.txt</t>
-  </si>
-  <si>
     <t>small locations: 2010, 2018</t>
   </si>
   <si>
@@ -169,33 +163,12 @@
     <t>all with non missing employer: 2007, 2010, 2018, 2019</t>
   </si>
   <si>
-    <t>year_area_job.txt</t>
-  </si>
-  <si>
-    <t>year_loc1_size.txt</t>
-  </si>
-  <si>
-    <t>year-location</t>
-  </si>
-  <si>
-    <t>year, location (latitude and longitude), number of job post at the given location in a given year</t>
-  </si>
-  <si>
-    <t>year, location (latitude and longitude), SOC occupation title_number of posts ((SOC1, # POST), (SOC2, # POST), ...)</t>
-  </si>
-  <si>
     <t>usmap/usa-states-census-2014.shp</t>
   </si>
   <si>
     <t>state geometry</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/holtzy/The-Python-Graph-Gallery/master/static/data/US-counties.geojson</t>
-  </si>
-  <si>
-    <t>county geometry</t>
-  </si>
-  <si>
     <t>2018_race_gender.xlsx</t>
   </si>
   <si>
@@ -310,25 +283,53 @@
     <t xml:space="preserve">all: 2010-2018 </t>
   </si>
   <si>
-    <t>all: 2010 and 2018</t>
+    <t>lcz_occ_year_skill_freq.txt</t>
+  </si>
+  <si>
+    <t>scz_occ_year_skill_freq.txt</t>
+  </si>
+  <si>
+    <t>ERS10.geojson</t>
+  </si>
+  <si>
+    <t>commuting zone geometry</t>
+  </si>
+  <si>
+    <t>year_jobid_cz_occ</t>
+  </si>
+  <si>
+    <t>year-jobid</t>
+  </si>
+  <si>
+    <t>all: 2018</t>
+  </si>
+  <si>
+    <t>year, jobid, commutizing zone, SOC occupation title</t>
+  </si>
+  <si>
+    <t>osvdedud_10perc821seed.txt</t>
+  </si>
+  <si>
+    <t>SOC-added skill number</t>
+  </si>
+  <si>
+    <t>Penn State University</t>
+  </si>
+  <si>
+    <t>random 10% of 2010</t>
+  </si>
+  <si>
+    <t>average skill vector distance, average education year difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,17 +358,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65776306-04D1-4FE5-84FA-2FA497EA1DCE}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,8 +720,8 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>93</v>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -736,10 +735,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -798,16 +797,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -815,7 +814,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -824,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -832,126 +831,126 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -960,161 +959,161 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>94</v>
+      <c r="D17" t="s">
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>94</v>
+      <c r="D18" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>54</v>
+      <c r="A20" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D21">
         <v>2018</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A20" r:id="rId1" xr:uid="{0B687389-DBDC-4153-9802-F705DBD7852C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1153,19 +1152,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1178,8 +1177,8 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>93</v>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1193,10 +1192,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -1221,7 +1220,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1230,15 +1229,15 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1247,7 +1246,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1255,24 +1254,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1281,74 +1280,74 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>2018</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>2018</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -1357,7 +1356,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1365,7 +1364,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -1374,7 +1373,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -1382,7 +1381,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1391,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -1399,7 +1398,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -1408,7 +1407,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -1416,7 +1415,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -1425,15 +1424,15 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -1442,10 +1441,10 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>